<commit_message>
Co-authored-by: Vinoth <Vinoth82003@users.noreply.github.com> admin.html
</commit_message>
<xml_diff>
--- a/app/static/excel/attendance_test.xlsx
+++ b/app/static/excel/attendance_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahav\OneDrive\Desktop\Projects\KKL-Attendance-System\app\static\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDesktop\Projects\KKL-Attendance-System\app\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0B1810C-84EE-46E4-94D3-A479CAEA8B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92EB94E-0B3F-4459-A4A3-77460DADA432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>emp_id</t>
   </si>
@@ -39,12 +39,6 @@
     <t>outtime</t>
   </si>
   <si>
-    <t>18:05</t>
-  </si>
-  <si>
-    <t>11:51</t>
-  </si>
-  <si>
     <t>20:26</t>
   </si>
   <si>
@@ -52,6 +46,9 @@
   </si>
   <si>
     <t>8A</t>
+  </si>
+  <si>
+    <t>8B</t>
   </si>
 </sst>
 </file>
@@ -152,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -167,6 +164,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,7 +550,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,13 +574,13 @@
         <v>101</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -590,13 +588,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>